<commit_message>
Organization Test case using Data Driven Framework
</commit_message>
<xml_diff>
--- a/src/com/vtiger/data/testdata.xlsx
+++ b/src/com/vtiger/data/testdata.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\home_practice\selenium_java\qspider\vtiger\src\com\vtiger\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C3C9E-391C-4EF4-A1F5-42A0788CBCD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="OrganizationInformation" sheetId="1" r:id="rId1"/>
+    <sheet name="AddressInformation" sheetId="2" r:id="rId2"/>
+    <sheet name="DescriptionInformation" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +26,115 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+  <si>
+    <t>Organization Name</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Ticker Symbol</t>
+  </si>
+  <si>
+    <t>Member Of</t>
+  </si>
+  <si>
+    <t>Employees</t>
+  </si>
+  <si>
+    <t>Other Email</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Email Opt Out</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Assigned To User</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Other Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Ownership</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>SIC Code</t>
+  </si>
+  <si>
+    <t>Annual Revenue</t>
+  </si>
+  <si>
+    <t>Notify Owner</t>
+  </si>
+  <si>
+    <t>Address Information</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing PO Box </t>
+  </si>
+  <si>
+    <t>Billing City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing State </t>
+  </si>
+  <si>
+    <t>Billing Postal Code</t>
+  </si>
+  <si>
+    <t>Billing Country</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Shipping PO Box</t>
+  </si>
+  <si>
+    <t>Shipping City</t>
+  </si>
+  <si>
+    <t>Shipping State</t>
+  </si>
+  <si>
+    <t>Shipping Postal Code</t>
+  </si>
+  <si>
+    <t>Shipping Country</t>
+  </si>
+  <si>
+    <t>Description Information</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +446,192 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1875E701-75E3-474A-BABC-EF39786939FA}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45213A0B-525D-4F83-9E20-ACA04CA0CD29}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>